<commit_message>
Update BOM & CPL
</commit_message>
<xml_diff>
--- a/PCBs/IRD_PCB_5/BOM_SMT_TB_RAK3172_868_IISS_PCB5.xlsx
+++ b/PCBs/IRD_PCB_5/BOM_SMT_TB_RAK3172_868_IISS_PCB5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Documents/TEX/Pau-05/PROJET-PRIMA-INTELIRRIS/PCBs/IRD-JFP/VRAK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0F4C2-910B-0E48-9CAC-C609167BA374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEABC51-E784-D241-AE0E-B83B9327292B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="780" windowWidth="24960" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="1460" windowWidth="24960" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_SMT_TB_RAK3172_868_IISS_PCB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Supplier Part</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C8,C1</t>
-  </si>
-  <si>
     <t>PZ254V-11-06P</t>
   </si>
   <si>
@@ -160,9 +154,6 @@
     <t>SMB(DO-214AA)</t>
   </si>
   <si>
-    <t>C113993</t>
-  </si>
-  <si>
     <t>R13,R7</t>
   </si>
   <si>
@@ -322,9 +313,6 @@
     <t>C22368237</t>
   </si>
   <si>
-    <t>C56372</t>
-  </si>
-  <si>
     <t>C146243</t>
   </si>
   <si>
@@ -344,6 +332,15 @@
   </si>
   <si>
     <t>C5188446</t>
+  </si>
+  <si>
+    <t>C841192</t>
+  </si>
+  <si>
+    <t>C473804</t>
+  </si>
+  <si>
+    <t>C1,C8</t>
   </si>
 </sst>
 </file>
@@ -827,8 +824,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1184,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,634 +1196,643 @@
     <col min="6" max="6" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1206</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="1">
+        <v>603</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>603</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>1206</v>
-      </c>
-      <c r="D2">
+      <c r="B9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1">
+        <v>603</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>603</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1">
+        <v>603</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1">
+        <v>603</v>
+      </c>
+      <c r="D19" s="1">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1">
+        <v>603</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1">
+        <v>603</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G2">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="1">
         <v>603</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
+      <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>603</v>
-      </c>
-      <c r="D5">
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6">
-        <v>10.1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="H8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>105</v>
-      </c>
-      <c r="J8" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9">
-        <v>0.40500000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10">
-        <v>0.245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11">
-        <v>5.5E-2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" t="s">
-        <v>99</v>
-      </c>
-      <c r="K11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13">
-        <v>0.86099999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14">
-        <v>0.114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16">
-        <v>603</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17">
-        <v>603</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>603</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19">
-        <v>603</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20">
-        <v>603</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23">
-        <v>603</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24">
-        <v>603</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>